<commit_message>
Setup folders for old code; start refactor
</commit_message>
<xml_diff>
--- a/DeterministicModel/Data/3xoxygraphData.xlsx
+++ b/DeterministicModel/Data/3xoxygraphData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t xml:space="preserve">Time [s]</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Light off, , </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On</t>
   </si>
   <si>
     <t xml:space="preserve">T 0.5</t>
@@ -152,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">Inhibit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off</t>
   </si>
 </sst>
 </file>
@@ -254,24 +260,23 @@
   </sheetPr>
   <dimension ref="A1:R705"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T4" activeCellId="0" sqref="T4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K691" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R706" activeCellId="0" sqref="R706"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1022" min="13" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,7 +392,9 @@
         <f aca="false">H2</f>
         <v>1.9406</v>
       </c>
-      <c r="R2" s="0"/>
+      <c r="R2" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -1226,10 +1233,10 @@
         <v>934</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>179.5293</v>
@@ -2582,10 +2589,10 @@
         <v>986</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>180.0532</v>
@@ -3314,10 +3321,10 @@
         <v>1014</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E59" s="1" t="n">
         <v>180.2777</v>
@@ -3994,10 +4001,10 @@
         <v>1040</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E72" s="1" t="n">
         <v>180.4074</v>
@@ -6858,10 +6865,10 @@
         <v>1150</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E127" s="1" t="n">
         <v>180.4174</v>
@@ -8734,10 +8741,10 @@
         <v>1222</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E163" s="1" t="n">
         <v>179.7039</v>
@@ -11598,10 +11605,10 @@
         <v>1332</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E218" s="1" t="n">
         <v>178.6812</v>
@@ -14306,10 +14313,10 @@
         <v>1436</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E270" s="1" t="n">
         <v>175.593</v>
@@ -18054,10 +18061,10 @@
         <v>1580</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E342" s="1" t="n">
         <v>148.822</v>
@@ -18156,7 +18163,7 @@
         <v>190.6427</v>
       </c>
       <c r="R343" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -20608,10 +20615,10 @@
         <v>1678</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C391" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E391" s="1" t="n">
         <v>126.3216</v>
@@ -20658,7 +20665,7 @@
         <v>204.789</v>
       </c>
       <c r="R391" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23786,10 +23793,10 @@
         <v>1800</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C452" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E452" s="1" t="n">
         <v>117.9999</v>
@@ -23836,7 +23843,7 @@
         <v>62.3049</v>
       </c>
       <c r="R452" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26236,10 +26243,10 @@
         <v>1894</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C499" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E499" s="1" t="n">
         <v>99.1565</v>
@@ -26286,7 +26293,7 @@
         <v>192.0216</v>
       </c>
       <c r="R499" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -29154,10 +29161,10 @@
         <v>2006</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C555" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E555" s="1" t="n">
         <v>65.5306</v>
@@ -29204,7 +29211,7 @@
         <v>281.3933</v>
       </c>
       <c r="R555" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31604,10 +31611,10 @@
         <v>2100</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C602" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E602" s="1" t="n">
         <v>33.2118</v>
@@ -31654,7 +31661,7 @@
         <v>316.8356</v>
       </c>
       <c r="R602" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33898,10 +33905,10 @@
         <v>2188</v>
       </c>
       <c r="B646" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C646" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E646" s="1" t="n">
         <v>5.2385</v>
@@ -33948,7 +33955,7 @@
         <v>304.3235</v>
       </c>
       <c r="R646" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36840,6 +36847,9 @@
       <c r="Q705" s="1" t="n">
         <f aca="false">H705</f>
         <v>-0.4086</v>
+      </c>
+      <c r="R705" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>